<commit_message>
wynegocjowano zakres do 100 w zamianie liczby na zapis tekstowy
</commit_message>
<xml_diff>
--- a/TextTransformer.xlsx
+++ b/TextTransformer.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27029"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://putpoznanpl-my.sharepoint.com/personal/aleksander_czarnecki_1_student_put_poznan_pl/Documents/SEMESTR 5/Inżynieria Oprogramowania/IOD-L09-Beta/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63C3B56A-A26D-4607-BF1B-1814A9B3878E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{63C3B56A-A26D-4607-BF1B-1814A9B3878E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4AA98A3F-39E7-4B9F-AF46-BC73A4B73782}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Opis" sheetId="3" r:id="rId1"/>
@@ -86,10 +86,6 @@
     <t>Jako użytkownik mogę zamieniać liczby na tekst w języku polskim (Wpłać 100 złotych -&gt; wpłać sto złotych) – wsparcie zakresu liczb do negocjacji</t>
   </si>
   <si>
-    <t>• zamiana liczb całkowitych do 1000
-• zamiana liczb zmiennoprzecinkowych do części setnych</t>
-  </si>
-  <si>
     <t>Jako użytkownik mogę o zamieniać wybrane (predefiniowane) słowa na skróty (Pieczywo to na przykład chleb i bułki -&gt; Pieczywo to np. chleb i bułki) – zakres obsługiwanych skrótów do negocjacji</t>
   </si>
   <si>
@@ -175,6 +171,10 @@
   </si>
   <si>
     <t>Integracja z REST API</t>
+  </si>
+  <si>
+    <t>• zamiana liczb całkowitych do 100
+• zamiana liczb zmiennoprzecinkowych do części setnych</t>
   </si>
 </sst>
 </file>
@@ -193,6 +193,8 @@
       <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -200,6 +202,8 @@
       <sz val="18"/>
       <color rgb="FF4F81BD"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -329,7 +333,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -789,17 +793,17 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="95.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" ht="23.4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="84.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" ht="84.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -818,20 +822,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="52" style="3" customWidth="1"/>
     <col min="2" max="2" width="15" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.25" style="4" customWidth="1"/>
-    <col min="4" max="4" width="25.375" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="58.125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="25.19921875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="25.3984375" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="58.09765625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -839,7 +843,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>11</v>
@@ -848,7 +852,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="63" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -865,7 +869,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="110.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="109.2" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
@@ -882,7 +886,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="63" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
@@ -899,7 +903,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
@@ -913,12 +917,12 @@
         <v>1</v>
       </c>
       <c r="E5" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="78" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>14</v>
       </c>
       <c r="B6" s="4">
         <v>10</v>
@@ -930,12 +934,12 @@
         <v>0.5</v>
       </c>
       <c r="E6" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="93.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>16</v>
       </c>
       <c r="B7" s="4">
         <v>10</v>
@@ -947,12 +951,12 @@
         <v>0.5</v>
       </c>
       <c r="E7" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>18</v>
       </c>
       <c r="B8" s="4">
         <v>2</v>
@@ -964,12 +968,12 @@
         <v>0.5</v>
       </c>
       <c r="E8" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="124.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="110.25" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>20</v>
       </c>
       <c r="B9" s="4">
         <v>1</v>
@@ -981,18 +985,18 @@
         <v>1</v>
       </c>
       <c r="E9" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>22</v>
       </c>
       <c r="C10" s="4">
         <v>160</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -1017,312 +1021,312 @@
       <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="45.125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="48.875" style="3" customWidth="1"/>
+    <col min="1" max="1" width="45.09765625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="48.8984375" style="3" customWidth="1"/>
     <col min="3" max="3" width="33" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="18" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C6" s="4">
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B7" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C7" s="4">
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B9" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C9" s="9">
         <f>SUM(C6:C7)</f>
         <v>150</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B12" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C12" s="4">
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B13" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C13" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B15" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C15" s="9">
         <f>SUM(C12:C13)</f>
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B18" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C18" s="4">
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B19" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C19" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B21" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C21" s="9">
         <f>SUM(C18:C19)</f>
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B24" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C24" s="4">
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B25" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C25" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B27" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C27" s="9">
         <f>SUM(C24:C25)</f>
         <v>30</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="63" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B30" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C30" s="4">
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B31" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C31" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B33" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C33" s="9">
         <f>SUM(C30:C31)</f>
         <v>30</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B36" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C36" s="4">
         <v>30</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B37" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C37" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B39" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C39" s="9">
         <f>SUM(C36:C37)</f>
         <v>40</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B42" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C42" s="11">
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B43" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C43" s="4">
         <v>50</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B44" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C44" s="4">
         <v>30</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B46" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C46" s="9">
         <f>SUM(C42:C44)</f>
         <v>120</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A48" s="12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B49" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C49" s="4">
         <v>70</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B50" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C50" s="4">
         <v>30</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B52" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C52" s="9">
         <f>SUM(C49:C50)</f>
         <v>100</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A54" s="12" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B55" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C55" s="4">
         <v>100</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B56" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C56" s="4">
         <v>30</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B57" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C57" s="4">
         <v>30</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B59" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C59" s="9">
         <f>SUM(C55:C57)</f>

</xml_diff>